<commit_message>
check sampling occurs 105ns after rising edge
</commit_message>
<xml_diff>
--- a/PIO_PDM.xlsx
+++ b/PIO_PDM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3229d0c75b2fab87/Documents/microPython/arduino nano rp2040 connect/pdm-microphone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{B618A679-2FBB-4F98-B4AD-8F31131AC995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBD31B05-E0F7-4045-901E-07D2250DFD84}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{B618A679-2FBB-4F98-B4AD-8F31131AC995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D375582A-39A0-469C-81BB-08797DCF8D7D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6D54BABA-A520-41FE-AC61-C599DD19A245}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="2.4MHz" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -690,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9602FD-D4B2-441A-AA0D-56428BC0A7C0}">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:G6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -993,53 +992,8 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="E23" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" t="s">
-        <v>52</v>
-      </c>
-      <c r="H23" t="s">
-        <v>52</v>
-      </c>
-      <c r="I23" t="s">
-        <v>52</v>
-      </c>
-      <c r="J23" t="s">
-        <v>52</v>
-      </c>
-      <c r="K23" t="s">
-        <v>52</v>
-      </c>
-      <c r="L23" t="s">
-        <v>52</v>
-      </c>
-      <c r="M23" t="s">
-        <v>52</v>
-      </c>
-      <c r="N23" t="s">
-        <v>52</v>
-      </c>
-      <c r="O23" t="s">
-        <v>52</v>
-      </c>
-      <c r="P23" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>52</v>
-      </c>
-      <c r="R23" t="s">
-        <v>52</v>
-      </c>
-      <c r="S23" t="s">
-        <v>52</v>
-      </c>
-      <c r="T23" t="s">
-        <v>52</v>
+      <c r="A23" s="12" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
@@ -1069,107 +1023,152 @@
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
-        <v>58</v>
+      <c r="D25" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D26" s="6" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="D27" s="6" t="s">
-        <v>64</v>
-      </c>
+      <c r="B27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="14"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="14"/>
+      <c r="M27" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="N27" s="15"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="14"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="14"/>
-      <c r="M28" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="N28" s="15"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="14"/>
+        <v>5</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="L28" s="14"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="K29" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="L29" s="14"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B30" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="S30" s="13" t="s">
+      <c r="S29" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="T30" s="14"/>
+      <c r="T29" s="14"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B31" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F31" s="14"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="14"/>
+      <c r="M31" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="N31" s="14"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B32" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F32" s="14"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="14"/>
-      <c r="M32" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="N32" s="14"/>
+        <v>5</v>
+      </c>
+      <c r="K32" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="L32" s="14"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B33" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="K33" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="L33" s="14"/>
+      <c r="O33" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P33" s="14"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="O34" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="P34" s="14"/>
+      <c r="Q34" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="R34" s="14"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="Q35" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="R35" s="14"/>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="Q36" s="9"/>
-      <c r="S36" s="13" t="s">
+      <c r="Q35" s="9"/>
+      <c r="S35" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="T36" s="14"/>
+      <c r="T35" s="14"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A37" s="12" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A38" s="12" t="s">
-        <v>57</v>
+      <c r="E38" t="s">
+        <v>52</v>
+      </c>
+      <c r="F38" t="s">
+        <v>52</v>
+      </c>
+      <c r="G38" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" t="s">
+        <v>52</v>
+      </c>
+      <c r="I38" t="s">
+        <v>52</v>
+      </c>
+      <c r="J38" t="s">
+        <v>52</v>
+      </c>
+      <c r="K38" t="s">
+        <v>52</v>
+      </c>
+      <c r="L38" t="s">
+        <v>52</v>
+      </c>
+      <c r="M38" t="s">
+        <v>52</v>
+      </c>
+      <c r="N38" t="s">
+        <v>52</v>
+      </c>
+      <c r="O38" t="s">
+        <v>52</v>
+      </c>
+      <c r="P38" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>52</v>
+      </c>
+      <c r="R38" t="s">
+        <v>52</v>
+      </c>
+      <c r="S38" t="s">
+        <v>52</v>
+      </c>
+      <c r="T38" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
check max freq attainable
</commit_message>
<xml_diff>
--- a/PIO_PDM.xlsx
+++ b/PIO_PDM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3229d0c75b2fab87/Documents/microPython/arduino nano rp2040 connect/pdm-microphone/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3229d0c75b2fab87/Documents/microPython/arduino nano rp2040 connect/mp34dt05-a-micropython-driver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{B618A679-2FBB-4F98-B4AD-8F31131AC995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D375582A-39A0-469C-81BB-08797DCF8D7D}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{B618A679-2FBB-4F98-B4AD-8F31131AC995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E2D33AF-7B89-4025-8ADE-173A4D702945}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6D54BABA-A520-41FE-AC61-C599DD19A245}"/>
   </bookViews>
@@ -689,14 +689,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9602FD-D4B2-441A-AA0D-56428BC0A7C0}">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="12.77734375" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
@@ -747,6 +748,7 @@
       <c r="E3" t="s">
         <v>20</v>
       </c>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.3">
       <c r="E4" s="2"/>

</xml_diff>